<commit_message>
modificaccion pantalla administracion productos
</commit_message>
<xml_diff>
--- a/Plantilla/TemplateProducto.xlsx
+++ b/Plantilla/TemplateProducto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tambours\OneDrive - Hewlett Packard Enterprise\Personal\Desarrollo\Repos\Cinderella\Plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stambour\OneDrive - DXC Production\Personal\Desarrollo\Repos\Cinderella\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -117,18 +117,6 @@
     <t>CodigoBarra</t>
   </si>
   <si>
-    <t>Efectivo_Tigre</t>
-  </si>
-  <si>
-    <t>Tarjeta_Tigre</t>
-  </si>
-  <si>
-    <t>Efectivo_Capital</t>
-  </si>
-  <si>
-    <t>Tarjeta_Capital</t>
-  </si>
-  <si>
     <t>Descripcion</t>
   </si>
   <si>
@@ -139,6 +127,18 @@
   </si>
   <si>
     <t>Mayorista</t>
+  </si>
+  <si>
+    <t>Lista_Tigre</t>
+  </si>
+  <si>
+    <t>Desc_Tigre</t>
+  </si>
+  <si>
+    <t>Lista_Capital</t>
+  </si>
+  <si>
+    <t>Desc_Capital</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -298,6 +298,10 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +612,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E9964" sqref="E9964"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,9 +631,9 @@
     <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="14" style="30" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="34" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="34" customWidth="1"/>
     <col min="15" max="15" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -668,28 +672,28 @@
         <v>9</v>
       </c>
       <c r="K1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="R1" s="24" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -703,9 +707,9 @@
       <c r="I2" s="18"/>
       <c r="J2" s="28"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="L2" s="32"/>
       <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
+      <c r="N2" s="32"/>
       <c r="O2" s="19"/>
       <c r="P2" s="20"/>
       <c r="Q2" s="13"/>
@@ -722,9 +726,9 @@
       <c r="I3" s="21"/>
       <c r="J3" s="29"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
+      <c r="L3" s="33"/>
       <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
+      <c r="N3" s="33"/>
       <c r="O3" s="22"/>
       <c r="P3" s="23"/>
       <c r="Q3" s="14"/>
@@ -741,9 +745,9 @@
       <c r="I4" s="21"/>
       <c r="J4" s="29"/>
       <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="L4" s="33"/>
       <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
+      <c r="N4" s="33"/>
       <c r="O4" s="22"/>
       <c r="P4" s="23"/>
       <c r="Q4" s="14"/>

</xml_diff>